<commit_message>
change data_util.py, recognize.py, main.py
</commit_message>
<xml_diff>
--- a/attend list.xlsx
+++ b/attend list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>HE170769</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-09-08 17:01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>HE123456</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2023-09-07 17:31:12</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-09-08 17:01:50</t>
         </is>
       </c>
     </row>

</xml_diff>